<commit_message>
Added validation to check for empty rows
</commit_message>
<xml_diff>
--- a/testFiles/Invalid Amount_2.xlsx
+++ b/testFiles/Invalid Amount_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tl_ch\Documents\SMU\SIS\Year 3.2\IS442 Object Oriented Programming\Project\Object-Orientated-Programming-G2Project\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yu Quan\Documents\Java\src\Project\Object-Orientated-Programming-G2Project\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A764B786-A74B-4F8E-ACB9-65EDE403C7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87775B0-5454-4383-A2E4-99931EE0C3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29145" yWindow="345" windowWidth="19425" windowHeight="10620" xr2:uid="{5F975919-C47D-ED4B-A3EE-295A5CBC72C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F975919-C47D-ED4B-A3EE-295A5CBC72C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction Details" sheetId="1" r:id="rId1"/>
@@ -670,7 +670,7 @@
     <t>XIAO MING</t>
   </si>
   <si>
-    <t>434dff</t>
+    <t>three thousand</t>
   </si>
 </sst>
 </file>
@@ -1377,35 +1377,35 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+      <selection activeCell="W1" sqref="W1:X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="50.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.69921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.83203125" customWidth="1"/>
-    <col min="17" max="17" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.796875" customWidth="1"/>
+    <col min="17" max="17" width="7.796875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="31.5" customWidth="1"/>
-    <col min="20" max="20" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.19921875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="45" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -1806,8 +1806,8 @@
       <c r="W6" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="X6" s="23">
-        <v>9000</v>
+      <c r="X6" s="23" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -2398,8 +2398,8 @@
       <c r="W14" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="X14" s="23" t="s">
-        <v>165</v>
+      <c r="X14" s="23">
+        <v>5000</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -2761,18 +2761,18 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="73.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="12.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.69921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.69921875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.19921875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.19921875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2801,7 +2801,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17">
+    <row r="2" spans="1:14" ht="17.399999999999999">
       <c r="A2" s="34" t="s">
         <v>29</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17">
+    <row r="3" spans="1:14" ht="17.399999999999999">
       <c r="A3" s="35"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -2857,7 +2857,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17">
+    <row r="4" spans="1:14" ht="17.399999999999999">
       <c r="A4" s="35"/>
       <c r="B4" s="7" t="s">
         <v>2</v>
@@ -2881,7 +2881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="62">
+    <row r="5" spans="1:14" ht="62.4">
       <c r="A5" s="35"/>
       <c r="B5" s="7" t="s">
         <v>3</v>
@@ -2905,7 +2905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17">
+    <row r="6" spans="1:14" ht="17.399999999999999">
       <c r="A6" s="35"/>
       <c r="B6" s="7" t="s">
         <v>7</v>
@@ -2929,7 +2929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17">
+    <row r="7" spans="1:14" ht="17.399999999999999">
       <c r="A7" s="35"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
@@ -2956,7 +2956,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17">
+    <row r="8" spans="1:14" ht="17.399999999999999">
       <c r="A8" s="35"/>
       <c r="B8" s="7" t="s">
         <v>9</v>
@@ -2983,7 +2983,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17">
+    <row r="9" spans="1:14" ht="17.399999999999999">
       <c r="A9" s="35"/>
       <c r="B9" s="7" t="s">
         <v>8</v>
@@ -3007,7 +3007,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17">
+    <row r="10" spans="1:14" ht="17.399999999999999">
       <c r="A10" s="35"/>
       <c r="B10" s="7" t="s">
         <v>10</v>
@@ -3032,7 +3032,7 @@
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="232.5">
+    <row r="11" spans="1:14" ht="234">
       <c r="A11" s="35"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
@@ -3056,7 +3056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="124">
+    <row r="12" spans="1:14" ht="124.8">
       <c r="A12" s="35"/>
       <c r="B12" s="7" t="s">
         <v>18</v>
@@ -3080,7 +3080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="170.5">
+    <row r="13" spans="1:14" ht="171.6">
       <c r="A13" s="35"/>
       <c r="B13" s="7" t="s">
         <v>11</v>
@@ -3104,7 +3104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="124">
+    <row r="14" spans="1:14" ht="124.8">
       <c r="A14" s="35"/>
       <c r="B14" s="7" t="s">
         <v>12</v>
@@ -3128,7 +3128,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17">
+    <row r="15" spans="1:14" ht="17.399999999999999">
       <c r="A15" s="36" t="s">
         <v>5</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="17">
+    <row r="16" spans="1:14" ht="17.399999999999999">
       <c r="A16" s="36"/>
       <c r="B16" s="7" t="s">
         <v>1</v>
@@ -3184,7 +3184,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17">
+    <row r="17" spans="1:9" ht="17.399999999999999">
       <c r="A17" s="36"/>
       <c r="B17" s="7" t="s">
         <v>2</v>
@@ -3208,7 +3208,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="62">
+    <row r="18" spans="1:9" ht="62.4">
       <c r="A18" s="36"/>
       <c r="B18" s="7" t="s">
         <v>3</v>
@@ -3232,7 +3232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17">
+    <row r="19" spans="1:9" ht="17.399999999999999">
       <c r="A19" s="36"/>
       <c r="B19" s="7" t="s">
         <v>7</v>
@@ -3256,7 +3256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="17">
+    <row r="20" spans="1:9" ht="17.399999999999999">
       <c r="A20" s="36"/>
       <c r="B20" s="7" t="s">
         <v>6</v>
@@ -3280,7 +3280,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17">
+    <row r="21" spans="1:9" ht="17.399999999999999">
       <c r="A21" s="36"/>
       <c r="B21" s="7" t="s">
         <v>4</v>
@@ -3307,7 +3307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17">
+    <row r="22" spans="1:9" ht="17.399999999999999">
       <c r="A22" s="36"/>
       <c r="B22" s="7" t="s">
         <v>8</v>
@@ -3331,7 +3331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17">
+    <row r="23" spans="1:9" ht="17.399999999999999">
       <c r="A23" s="36"/>
       <c r="B23" s="7" t="s">
         <v>10</v>
@@ -3355,7 +3355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17" customHeight="1">
+    <row r="24" spans="1:9" ht="16.95" customHeight="1">
       <c r="A24" s="37" t="s">
         <v>16</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17" customHeight="1">
+    <row r="25" spans="1:9" ht="16.95" customHeight="1">
       <c r="A25" s="37"/>
       <c r="B25" s="7" t="s">
         <v>34</v>
@@ -3408,7 +3408,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17">
+    <row r="26" spans="1:9" ht="17.399999999999999">
       <c r="A26" s="38" t="s">
         <v>41</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="17">
+    <row r="27" spans="1:9" ht="17.399999999999999">
       <c r="A27" s="38"/>
       <c r="B27" s="7" t="s">
         <v>42</v>

</xml_diff>